<commit_message>
task 3 done, task 4 almost done
</commit_message>
<xml_diff>
--- a/Game Business Studies/task 4/ICT-Gap-Analysis-Template.xlsx
+++ b/Game Business Studies/task 4/ICT-Gap-Analysis-Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sync\AIELaptop\AIE\2021\Content\Professional-Studies-2\Topics\Assessment Briefs\Assessment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s231135\GitHub\Robert-2\Game Business Studies\task 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABFE1E2F-3B90-4839-A1E9-4D45064F9D1C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{731A766C-0C92-4747-BC49-BDF3771CDB88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Document History" sheetId="4" r:id="rId1"/>
@@ -45,18 +45,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="113">
   <si>
     <t>First Draft</t>
   </si>
   <si>
     <t>j. Smith</t>
-  </si>
-  <si>
-    <t>Example Row</t>
-  </si>
-  <si>
-    <t>Example Text</t>
   </si>
   <si>
     <t>NOTES</t>
@@ -96,18 +90,12 @@
     <t>COMPLETE</t>
   </si>
   <si>
-    <t>Regular cleaning by staff to prevent rotten food</t>
-  </si>
-  <si>
     <t>J. Smith</t>
   </si>
   <si>
     <t>NO</t>
   </si>
   <si>
-    <t>100% on-time delivery</t>
-  </si>
-  <si>
     <t>HIGH</t>
   </si>
   <si>
@@ -129,9 +117,6 @@
     <t>Using personal licenses for all software</t>
   </si>
   <si>
-    <t>Example notes</t>
-  </si>
-  <si>
     <t>HARDWARE GAP ANALYSIS</t>
   </si>
   <si>
@@ -180,9 +165,6 @@
     <t>One personally owned Oculus Rift, attached to Facebook account</t>
   </si>
   <si>
-    <t>Install Unity Hub &amp; Unity 2020.1.10 on all machines</t>
-  </si>
-  <si>
     <t>Install Unreal Marketplace and UE4 4.26 on all machines</t>
   </si>
   <si>
@@ -264,9 +246,6 @@
     <t>All staff</t>
   </si>
   <si>
-    <t>New staff &amp; constractors</t>
-  </si>
-  <si>
     <t>WHO'S AFFECTED?</t>
   </si>
   <si>
@@ -280,6 +259,132 @@
   </si>
   <si>
     <t>Team members using own devices</t>
+  </si>
+  <si>
+    <t>Evaluate Maya licensing for artists</t>
+  </si>
+  <si>
+    <t>Update all machines to use Windows 10 Enterprise</t>
+  </si>
+  <si>
+    <t>Evaluate Hack'n'Plan for use instead of Trello</t>
+  </si>
+  <si>
+    <t>Mobile Phone Test Devices provided for use</t>
+  </si>
+  <si>
+    <t>Suitable Anti-Virus provided on all devices</t>
+  </si>
+  <si>
+    <t>Purchase phone(s) for use as Test Device(s)</t>
+  </si>
+  <si>
+    <t>Research suitable options for Anti-Virus</t>
+  </si>
+  <si>
+    <t>Train employees to be vigilant against viruses</t>
+  </si>
+  <si>
+    <t>Evaluate Google Docs for use, with shared repository</t>
+  </si>
+  <si>
+    <t>Upgrade Office.com student accounts to business accounts</t>
+  </si>
+  <si>
+    <t>Evaluate Blender for artists</t>
+  </si>
+  <si>
+    <t>Upgrade to Trello Premium</t>
+  </si>
+  <si>
+    <t>Rent out Mobile Phone(s) for use as Test Device(s)</t>
+  </si>
+  <si>
+    <t>Company owned Oculus Rift, attached to Company account</t>
+  </si>
+  <si>
+    <t>Company Wifi</t>
+  </si>
+  <si>
+    <t>Keycards for existing team members, plus temporary and guest cards, access during business hours</t>
+  </si>
+  <si>
+    <t>New staff &amp; constractors, All staff</t>
+  </si>
+  <si>
+    <t>Daily backups to source control, weekly backups to external HDD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Install Unity Hub &amp; Unity 2020.1.10 on all machines </t>
+  </si>
+  <si>
+    <t>All staff have personal workstation</t>
+  </si>
+  <si>
+    <t>Additional storage</t>
+  </si>
+  <si>
+    <t>Rent Offsite server</t>
+  </si>
+  <si>
+    <t>Alter current systems to allow for temporary passes and less access hours</t>
+  </si>
+  <si>
+    <t>Evaluate new system that allows for desired features</t>
+  </si>
+  <si>
+    <t>Company-provided passwords that change monthly</t>
+  </si>
+  <si>
+    <t>Shared, single cloud service</t>
+  </si>
+  <si>
+    <t>Purchase onsite PCs for all staff</t>
+  </si>
+  <si>
+    <t>Purchase company laptops for all staff</t>
+  </si>
+  <si>
+    <t>Second Draft</t>
+  </si>
+  <si>
+    <t>E. Hurst</t>
+  </si>
+  <si>
+    <t>Evaluate Github for storage use</t>
+  </si>
+  <si>
+    <t>Evaluate Perforce for storage use</t>
+  </si>
+  <si>
+    <t>Purchase and maintain onsite server</t>
+  </si>
+  <si>
+    <t>Purchase Oculus Rift and make company account</t>
+  </si>
+  <si>
+    <t>Evaluate plausibilty of obtaining an Oculus Dev kit</t>
+  </si>
+  <si>
+    <t>Evaluate company-wide Wifi plan</t>
+  </si>
+  <si>
+    <t>Evaluate Separate wifi plan for artists, designers, programmers etc.</t>
+  </si>
+  <si>
+    <t>Evaluate system for automatically providing randomised passwords</t>
+  </si>
+  <si>
+    <t>Manually design secure passwords for employees, monthly</t>
+  </si>
+  <si>
+    <t>Evaluate use of a company Google Drive</t>
+  </si>
+  <si>
+    <t>Evaluate use of a company Onedrive</t>
+  </si>
+  <si>
+    <t>Update all machines to use Windows 10/11 Pro</t>
   </si>
 </sst>
 </file>
@@ -512,10 +617,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -579,9 +684,6 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -597,13 +699,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -612,6 +713,34 @@
     <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
   </cellStyles>
   <dxfs count="45">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE2EAF2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE2EAF2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1032,20 +1161,6 @@
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE2EAF2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -1460,20 +1575,6 @@
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE2EAF2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1708,7 +1809,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Maintenance Work Order"/>
@@ -1739,38 +1840,38 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B5EAFAC3-6F8A-4737-9FBF-2A28E836C988}" name="Table3" displayName="Table3" ref="B2:L28" totalsRowShown="0" headerRowDxfId="32" dataDxfId="30" headerRowBorderDxfId="31" tableBorderDxfId="29" totalsRowBorderDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B5EAFAC3-6F8A-4737-9FBF-2A28E836C988}" name="Table3" displayName="Table3" ref="B2:L28" totalsRowShown="0" headerRowDxfId="34" dataDxfId="32" headerRowBorderDxfId="33" tableBorderDxfId="31" totalsRowBorderDxfId="30">
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{F3757580-5D27-490D-B976-1F5F199C6D65}" name="REF NO." dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{9FAD9991-BC18-4AE0-BA57-7FDC3C8C1228}" name="ITEM" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{4BA6B1CD-DE66-455D-9E1E-E81A34D8005A}" name="CURRENT STATE" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{C81C3A38-F086-4011-9383-3B069BE7B41D}" name="DESIRED STATE" dataDxfId="24"/>
-    <tableColumn id="9" xr3:uid="{81C1643D-96D2-414A-A9E4-F6E86F699875}" name="PRIORITY" dataDxfId="23"/>
-    <tableColumn id="7" xr3:uid="{89CC30F0-5818-4832-8B22-946B36F15EA2}" name="WHO'S AFFECTED?" dataDxfId="22"/>
-    <tableColumn id="6" xr3:uid="{98BF8708-63C2-4919-8954-3DC1B0F0DB8C}" name="OPTION 1" dataDxfId="21"/>
-    <tableColumn id="11" xr3:uid="{CA1665D5-6E31-4232-AF86-6716DD9ED11D}" name="OPTION 2 (Alternative)" dataDxfId="20"/>
-    <tableColumn id="13" xr3:uid="{96AD023E-ADD1-4441-96DB-73F626CC6166}" name="ASSIGNED _x000a_TO" dataDxfId="19"/>
-    <tableColumn id="5" xr3:uid="{A1AF9E7E-3C8F-467C-A771-10DF5F0136E9}" name="COMPLETE" dataDxfId="18"/>
-    <tableColumn id="12" xr3:uid="{670D4632-259B-4C9C-9321-54194EC0926A}" name="NOTES" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{F3757580-5D27-490D-B976-1F5F199C6D65}" name="REF NO." dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{9FAD9991-BC18-4AE0-BA57-7FDC3C8C1228}" name="ITEM" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{4BA6B1CD-DE66-455D-9E1E-E81A34D8005A}" name="CURRENT STATE" dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{C81C3A38-F086-4011-9383-3B069BE7B41D}" name="DESIRED STATE" dataDxfId="26"/>
+    <tableColumn id="9" xr3:uid="{81C1643D-96D2-414A-A9E4-F6E86F699875}" name="PRIORITY" dataDxfId="25"/>
+    <tableColumn id="7" xr3:uid="{89CC30F0-5818-4832-8B22-946B36F15EA2}" name="WHO'S AFFECTED?" dataDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{98BF8708-63C2-4919-8954-3DC1B0F0DB8C}" name="OPTION 1" dataDxfId="23"/>
+    <tableColumn id="11" xr3:uid="{CA1665D5-6E31-4232-AF86-6716DD9ED11D}" name="OPTION 2 (Alternative)" dataDxfId="22"/>
+    <tableColumn id="13" xr3:uid="{96AD023E-ADD1-4441-96DB-73F626CC6166}" name="ASSIGNED _x000a_TO" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{A1AF9E7E-3C8F-467C-A771-10DF5F0136E9}" name="COMPLETE" dataDxfId="20"/>
+    <tableColumn id="12" xr3:uid="{670D4632-259B-4C9C-9321-54194EC0926A}" name="NOTES" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="B2:L28" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="B2:L28" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16" totalsRowBorderDxfId="15">
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="REF NO." dataDxfId="10"/>
-    <tableColumn id="11" xr3:uid="{167B9645-77DA-446A-A8A2-43EC0905C5B7}" name="ITEM" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="CURRENT STATE" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="DESIRED STATE" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{A88EF44B-853F-4BA4-BE69-5F15E5E185F0}" name="PRIORITY" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{4D373E46-7577-4C1F-8D5F-C0D657691EB7}" name="WHO'S AFFECTED?" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="OPTION 1" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="OPTION 2 (Alternative)" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{270E592A-E1ED-4F82-AF29-3532DDBD1B24}" name="ASSIGNED _x000a_TO" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{CF7A235F-E82F-4A4F-B022-C713D11CB827}" name="COMPLETE" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="NOTES" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="REF NO." dataDxfId="14"/>
+    <tableColumn id="11" xr3:uid="{167B9645-77DA-446A-A8A2-43EC0905C5B7}" name="ITEM" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="CURRENT STATE" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="DESIRED STATE" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{A88EF44B-853F-4BA4-BE69-5F15E5E185F0}" name="PRIORITY" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{4D373E46-7577-4C1F-8D5F-C0D657691EB7}" name="WHO'S AFFECTED?" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="OPTION 1" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="OPTION 2 (Alternative)" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{270E592A-E1ED-4F82-AF29-3532DDBD1B24}" name="ASSIGNED _x000a_TO" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{CF7A235F-E82F-4A4F-B022-C713D11CB827}" name="COMPLETE" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="NOTES" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2105,7 +2206,7 @@
   <dimension ref="B1:F14"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2121,7 +2222,7 @@
   <sheetData>
     <row r="1" spans="2:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="19" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C1" s="18"/>
       <c r="D1" s="18"/>
@@ -2130,24 +2231,24 @@
     </row>
     <row r="2" spans="2:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="17" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="2:6" s="1" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="14">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C3" s="13">
         <v>41255</v>
@@ -2158,15 +2259,21 @@
       <c r="E3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="11" t="s">
-        <v>2</v>
-      </c>
+      <c r="F3" s="11"/>
     </row>
     <row r="4" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="10"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
+      <c r="B4" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="C4" s="9">
+        <v>45597</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>100</v>
+      </c>
       <c r="F4" s="7"/>
     </row>
     <row r="5" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2256,11 +2363,11 @@
   </sheetPr>
   <dimension ref="B1:L28"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomRight" activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2270,7 +2377,7 @@
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="5" width="24.875" customWidth="1"/>
     <col min="6" max="6" width="9.625" customWidth="1"/>
-    <col min="7" max="7" width="14.25" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
     <col min="8" max="9" width="27.375" customWidth="1"/>
     <col min="10" max="10" width="10.375" customWidth="1"/>
     <col min="11" max="11" width="10.5" customWidth="1"/>
@@ -2279,544 +2386,619 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
+      <c r="B1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
-      <c r="J1" s="24"/>
+      <c r="J1" s="2"/>
     </row>
     <row r="2" spans="2:12" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="21" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C2" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="22" t="s">
+      <c r="G2" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="J2" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="K2" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="23" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" s="30" customFormat="1" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="B3" s="24">
+        <v>1</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="F3" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="I3" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="J3" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="H2" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="I2" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="J2" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="L2" s="23" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="2:12" s="31" customFormat="1" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="B3" s="25">
-        <v>1</v>
-      </c>
-      <c r="C3" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="26" t="s">
-        <v>71</v>
-      </c>
-      <c r="H3" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="I3" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="J3" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="L3" s="27" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" s="31" customFormat="1" ht="27" x14ac:dyDescent="0.25">
-      <c r="B4" s="25">
+      <c r="K3" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="L3" s="26"/>
+    </row>
+    <row r="4" spans="2:12" s="30" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+      <c r="B4" s="24">
         <f>B3+1</f>
         <v>2</v>
       </c>
-      <c r="C4" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" s="26" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="I4" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="J4" s="26" t="s">
+      <c r="C4" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="F4" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="L4" s="27" t="s">
-        <v>27</v>
-      </c>
+      <c r="G4" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="H4" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="I4" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="J4" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" s="26"/>
     </row>
     <row r="5" spans="2:12" ht="40.5" x14ac:dyDescent="0.25">
       <c r="B5" s="20">
         <f t="shared" ref="B5:B28" si="0">B4+1</f>
         <v>3</v>
       </c>
-      <c r="C5" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="27"/>
+      <c r="C5" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="F5" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="H5" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="I5" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="J5" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" s="26"/>
     </row>
     <row r="6" spans="2:12" ht="40.5" x14ac:dyDescent="0.25">
       <c r="B6" s="20">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C6" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="26"/>
-      <c r="L6" s="27"/>
-    </row>
-    <row r="7" spans="2:12" ht="27" x14ac:dyDescent="0.25">
+      <c r="C6" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="F6" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="H6" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="I6" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="J6" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" s="26"/>
+    </row>
+    <row r="7" spans="2:12" ht="40.5" x14ac:dyDescent="0.25">
       <c r="B7" s="20">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C7" s="26" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="26"/>
-      <c r="L7" s="27"/>
-    </row>
-    <row r="8" spans="2:12" ht="27" x14ac:dyDescent="0.25">
+      <c r="C7" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="F7" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="H7" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="I7" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="J7" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="L7" s="26"/>
+    </row>
+    <row r="8" spans="2:12" ht="54" x14ac:dyDescent="0.25">
       <c r="B8" s="20">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C8" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="D8" s="26" t="s">
+      <c r="C8" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="F8" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="H8" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="I8" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="J8" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="L8" s="26"/>
+    </row>
+    <row r="9" spans="2:12" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="B9" s="20">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="F9" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26" t="s">
-        <v>72</v>
-      </c>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="26"/>
-      <c r="L8" s="27"/>
-    </row>
-    <row r="9" spans="2:12" ht="27" x14ac:dyDescent="0.25">
-      <c r="B9" s="20">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="C9" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="D9" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="26"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="27"/>
+      <c r="H9" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="I9" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="J9" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="L9" s="26"/>
     </row>
     <row r="10" spans="2:12" ht="27" x14ac:dyDescent="0.25">
       <c r="B10" s="20">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C10" s="26" t="s">
-        <v>68</v>
-      </c>
-      <c r="D10" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="E10" s="26"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="26"/>
-      <c r="L10" s="27"/>
+      <c r="C10" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="F10" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="H10" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="I10" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="J10" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="K10" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="L10" s="26"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" s="20">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="26"/>
-      <c r="L11" s="27"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="26"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" s="20">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
-      <c r="K12" s="26"/>
-      <c r="L12" s="27"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="26"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" s="20">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="26"/>
-      <c r="K13" s="26"/>
-      <c r="L13" s="27"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="25"/>
+      <c r="L13" s="26"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" s="20">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="26"/>
-      <c r="K14" s="26"/>
-      <c r="L14" s="27"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="25"/>
+      <c r="L14" s="26"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" s="20">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="26"/>
-      <c r="K15" s="26"/>
-      <c r="L15" s="27"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="25"/>
+      <c r="K15" s="25"/>
+      <c r="L15" s="26"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" s="20">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="26"/>
-      <c r="L16" s="27"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="25"/>
+      <c r="L16" s="26"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="20">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
-      <c r="K17" s="26"/>
-      <c r="L17" s="27"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="25"/>
+      <c r="K17" s="25"/>
+      <c r="L17" s="26"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" s="20">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
-      <c r="K18" s="26"/>
-      <c r="L18" s="27"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="25"/>
+      <c r="J18" s="25"/>
+      <c r="K18" s="25"/>
+      <c r="L18" s="26"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="20">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="26"/>
-      <c r="K19" s="26"/>
-      <c r="L19" s="27"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="25"/>
+      <c r="J19" s="25"/>
+      <c r="K19" s="25"/>
+      <c r="L19" s="26"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" s="20">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
-      <c r="K20" s="26"/>
-      <c r="L20" s="27"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="25"/>
+      <c r="K20" s="25"/>
+      <c r="L20" s="26"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" s="20">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="26"/>
-      <c r="J21" s="26"/>
-      <c r="K21" s="26"/>
-      <c r="L21" s="27"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="25"/>
+      <c r="J21" s="25"/>
+      <c r="K21" s="25"/>
+      <c r="L21" s="26"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B22" s="20">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="26"/>
-      <c r="J22" s="26"/>
-      <c r="K22" s="26"/>
-      <c r="L22" s="27"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="25"/>
+      <c r="I22" s="25"/>
+      <c r="J22" s="25"/>
+      <c r="K22" s="25"/>
+      <c r="L22" s="26"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23" s="20">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="26"/>
-      <c r="I23" s="26"/>
-      <c r="J23" s="26"/>
-      <c r="K23" s="26"/>
-      <c r="L23" s="27"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="25"/>
+      <c r="I23" s="25"/>
+      <c r="J23" s="25"/>
+      <c r="K23" s="25"/>
+      <c r="L23" s="26"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B24" s="20">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="26"/>
-      <c r="J24" s="26"/>
-      <c r="K24" s="26"/>
-      <c r="L24" s="27"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="25"/>
+      <c r="I24" s="25"/>
+      <c r="J24" s="25"/>
+      <c r="K24" s="25"/>
+      <c r="L24" s="26"/>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B25" s="20">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="26"/>
-      <c r="J25" s="26"/>
-      <c r="K25" s="26"/>
-      <c r="L25" s="27"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="25"/>
+      <c r="I25" s="25"/>
+      <c r="J25" s="25"/>
+      <c r="K25" s="25"/>
+      <c r="L25" s="26"/>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B26" s="20">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="26"/>
-      <c r="H26" s="26"/>
-      <c r="I26" s="26"/>
-      <c r="J26" s="26"/>
-      <c r="K26" s="26"/>
-      <c r="L26" s="27"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="25"/>
+      <c r="I26" s="25"/>
+      <c r="J26" s="25"/>
+      <c r="K26" s="25"/>
+      <c r="L26" s="26"/>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B27" s="20">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="26"/>
-      <c r="H27" s="26"/>
-      <c r="I27" s="26"/>
-      <c r="J27" s="26"/>
-      <c r="K27" s="26"/>
-      <c r="L27" s="27"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="25"/>
+      <c r="G27" s="25"/>
+      <c r="H27" s="25"/>
+      <c r="I27" s="25"/>
+      <c r="J27" s="25"/>
+      <c r="K27" s="25"/>
+      <c r="L27" s="26"/>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B28" s="20">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="C28" s="28"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="28"/>
-      <c r="K28" s="28"/>
-      <c r="L28" s="29"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="27"/>
+      <c r="I28" s="27"/>
+      <c r="J28" s="27"/>
+      <c r="K28" s="27"/>
+      <c r="L28" s="28"/>
     </row>
   </sheetData>
   <phoneticPr fontId="10" type="noConversion"/>
   <conditionalFormatting sqref="K3:K28">
-    <cfRule type="containsText" dxfId="34" priority="1" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",K3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="2" operator="containsText" text="YES">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH("YES",K3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5:I28" xr:uid="{902461CF-2D74-45B6-80ED-B5762F3F11D0}">
-      <formula1>#REF!</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.3" right="0.3" top="0.3" bottom="0.3" header="0" footer="0"/>
   <pageSetup scale="58" fitToHeight="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <tableParts count="1">
@@ -2851,11 +3033,11 @@
   </sheetPr>
   <dimension ref="B1:L28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomRight" activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2873,562 +3055,619 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
+      <c r="B1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
-      <c r="J1" s="24"/>
+      <c r="J1" s="2"/>
     </row>
     <row r="2" spans="2:12" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="21" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C2" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="22" t="s">
+      <c r="G2" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="J2" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="K2" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="23" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" s="29" customFormat="1" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="B3" s="24">
+        <v>1</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="I3" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="J3" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="H2" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="I2" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="J2" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="L2" s="23" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="2:12" s="30" customFormat="1" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="B3" s="25">
-        <v>1</v>
-      </c>
-      <c r="C3" s="26" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="26" t="s">
-        <v>71</v>
-      </c>
-      <c r="H3" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="I3" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="J3" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="L3" s="27" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" s="30" customFormat="1" ht="27" x14ac:dyDescent="0.25">
-      <c r="B4" s="25">
+      <c r="K3" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="L3" s="26"/>
+    </row>
+    <row r="4" spans="2:12" s="29" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+      <c r="B4" s="24">
         <f>B3+1</f>
         <v>2</v>
       </c>
-      <c r="C4" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="26" t="s">
+      <c r="C4" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="I4" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="J4" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="K4" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="L4" s="27"/>
-    </row>
-    <row r="5" spans="2:12" s="32" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+      <c r="F4" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="H4" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="L4" s="26"/>
+    </row>
+    <row r="5" spans="2:12" ht="27" x14ac:dyDescent="0.25">
       <c r="B5" s="20">
         <f t="shared" ref="B5:B28" si="0">B4+1</f>
         <v>3</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="H5" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="I5" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="J5" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" s="26"/>
+    </row>
+    <row r="6" spans="2:12" ht="27" x14ac:dyDescent="0.25">
+      <c r="B6" s="20">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="H6" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="I6" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="J6" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" s="26"/>
+    </row>
+    <row r="7" spans="2:12" ht="27" x14ac:dyDescent="0.25">
+      <c r="B7" s="20">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="H7" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="I7" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="J7" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="L7" s="26"/>
+    </row>
+    <row r="8" spans="2:12" ht="27" x14ac:dyDescent="0.25">
+      <c r="B8" s="20">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="F8" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="H8" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="I8" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="J8" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="L8" s="26"/>
+    </row>
+    <row r="9" spans="2:12" ht="27" x14ac:dyDescent="0.25">
+      <c r="B9" s="20">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="H9" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="I9" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="J9" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="L9" s="26"/>
+    </row>
+    <row r="10" spans="2:12" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="B10" s="20">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="D5" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="E5" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" s="26" t="s">
+      <c r="E10" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="H10" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="I10" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="J10" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="K10" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="L10" s="26"/>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="20">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="26"/>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="20">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="26"/>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="20">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="25"/>
+      <c r="L13" s="26"/>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B14" s="20">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="25"/>
+      <c r="L14" s="26"/>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B15" s="20">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="25"/>
+      <c r="K15" s="25"/>
+      <c r="L15" s="26"/>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="20">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="25"/>
+      <c r="L16" s="26"/>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B17" s="20">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="25"/>
+      <c r="K17" s="25"/>
+      <c r="L17" s="26"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B18" s="20">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="25"/>
+      <c r="J18" s="25"/>
+      <c r="K18" s="25"/>
+      <c r="L18" s="26"/>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B19" s="20">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="25"/>
+      <c r="J19" s="25"/>
+      <c r="K19" s="25"/>
+      <c r="L19" s="26"/>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B20" s="20">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="25"/>
+      <c r="K20" s="25"/>
+      <c r="L20" s="26"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B21" s="20">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="25"/>
+      <c r="J21" s="25"/>
+      <c r="K21" s="25"/>
+      <c r="L21" s="26"/>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B22" s="20">
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="G5" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="L5" s="27"/>
-    </row>
-    <row r="6" spans="2:12" s="32" customFormat="1" ht="27" x14ac:dyDescent="0.25">
-      <c r="B6" s="20">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="C6" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="E6" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="26" t="s">
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="25"/>
+      <c r="I22" s="25"/>
+      <c r="J22" s="25"/>
+      <c r="K22" s="25"/>
+      <c r="L22" s="26"/>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B23" s="20">
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="L6" s="27"/>
-    </row>
-    <row r="7" spans="2:12" s="32" customFormat="1" ht="27" x14ac:dyDescent="0.25">
-      <c r="B7" s="20">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C7" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="D7" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26" t="s">
-        <v>71</v>
-      </c>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="26"/>
-      <c r="L7" s="27"/>
-    </row>
-    <row r="8" spans="2:12" s="32" customFormat="1" ht="27" x14ac:dyDescent="0.25">
-      <c r="B8" s="20">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="C8" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="D8" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="26"/>
-      <c r="L8" s="27"/>
-    </row>
-    <row r="9" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="20">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="C9" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="D9" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="26"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="27"/>
-    </row>
-    <row r="10" spans="2:12" s="32" customFormat="1" ht="27" x14ac:dyDescent="0.25">
-      <c r="B10" s="20">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="C10" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="D10" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="E10" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="26"/>
-      <c r="L10" s="27"/>
-    </row>
-    <row r="11" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="20">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="26"/>
-      <c r="L11" s="27"/>
-    </row>
-    <row r="12" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="20">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
-      <c r="K12" s="26"/>
-      <c r="L12" s="27"/>
-    </row>
-    <row r="13" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="20">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="26"/>
-      <c r="K13" s="26"/>
-      <c r="L13" s="27"/>
-    </row>
-    <row r="14" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="20">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="26"/>
-      <c r="K14" s="26"/>
-      <c r="L14" s="27"/>
-    </row>
-    <row r="15" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="20">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="26"/>
-      <c r="K15" s="26"/>
-      <c r="L15" s="27"/>
-    </row>
-    <row r="16" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="20">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="26"/>
-      <c r="L16" s="27"/>
-    </row>
-    <row r="17" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="20">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
-      <c r="K17" s="26"/>
-      <c r="L17" s="27"/>
-    </row>
-    <row r="18" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="20">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
-      <c r="K18" s="26"/>
-      <c r="L18" s="27"/>
-    </row>
-    <row r="19" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="20">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="26"/>
-      <c r="K19" s="26"/>
-      <c r="L19" s="27"/>
-    </row>
-    <row r="20" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="20">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
-      <c r="K20" s="26"/>
-      <c r="L20" s="27"/>
-    </row>
-    <row r="21" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="20">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="26"/>
-      <c r="J21" s="26"/>
-      <c r="K21" s="26"/>
-      <c r="L21" s="27"/>
-    </row>
-    <row r="22" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="20">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="26"/>
-      <c r="J22" s="26"/>
-      <c r="K22" s="26"/>
-      <c r="L22" s="27"/>
-    </row>
-    <row r="23" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="20">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="26"/>
-      <c r="I23" s="26"/>
-      <c r="J23" s="26"/>
-      <c r="K23" s="26"/>
-      <c r="L23" s="27"/>
-    </row>
-    <row r="24" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C23" s="25"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="25"/>
+      <c r="I23" s="25"/>
+      <c r="J23" s="25"/>
+      <c r="K23" s="25"/>
+      <c r="L23" s="26"/>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B24" s="20">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="26"/>
-      <c r="J24" s="26"/>
-      <c r="K24" s="26"/>
-      <c r="L24" s="27"/>
-    </row>
-    <row r="25" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="25"/>
+      <c r="I24" s="25"/>
+      <c r="J24" s="25"/>
+      <c r="K24" s="25"/>
+      <c r="L24" s="26"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B25" s="20">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="26"/>
-      <c r="J25" s="26"/>
-      <c r="K25" s="26"/>
-      <c r="L25" s="27"/>
-    </row>
-    <row r="26" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="25"/>
+      <c r="I25" s="25"/>
+      <c r="J25" s="25"/>
+      <c r="K25" s="25"/>
+      <c r="L25" s="26"/>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B26" s="20">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="26"/>
-      <c r="H26" s="26"/>
-      <c r="I26" s="26"/>
-      <c r="J26" s="26"/>
-      <c r="K26" s="26"/>
-      <c r="L26" s="27"/>
-    </row>
-    <row r="27" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C26" s="25"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="25"/>
+      <c r="I26" s="25"/>
+      <c r="J26" s="25"/>
+      <c r="K26" s="25"/>
+      <c r="L26" s="26"/>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B27" s="20">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="26"/>
-      <c r="H27" s="26"/>
-      <c r="I27" s="26"/>
-      <c r="J27" s="26"/>
-      <c r="K27" s="26"/>
-      <c r="L27" s="27"/>
-    </row>
-    <row r="28" spans="2:12" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C27" s="25"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="25"/>
+      <c r="G27" s="25"/>
+      <c r="H27" s="25"/>
+      <c r="I27" s="25"/>
+      <c r="J27" s="25"/>
+      <c r="K27" s="25"/>
+      <c r="L27" s="26"/>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B28" s="20">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="C28" s="28"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="28"/>
-      <c r="K28" s="28"/>
-      <c r="L28" s="29"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="27"/>
+      <c r="I28" s="27"/>
+      <c r="J28" s="27"/>
+      <c r="K28" s="27"/>
+      <c r="L28" s="28"/>
     </row>
   </sheetData>
   <phoneticPr fontId="10" type="noConversion"/>
   <conditionalFormatting sqref="K3:K28">
-    <cfRule type="containsText" dxfId="16" priority="1" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",K3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="2" operator="containsText" text="YES">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH("YES",K3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5:I28" xr:uid="{CFCC56A9-F04E-4187-B22B-FC9E4B1205F5}">
-      <formula1>#REF!</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.3" right="0.3" top="0.3" bottom="0.3" header="0" footer="0"/>
   <pageSetup scale="69" fitToHeight="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <tableParts count="1">
@@ -3436,7 +3675,7 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1DF0FB05-06F9-4AEB-B0CD-E1900E898650}">
           <x14:formula1>
             <xm:f>Ref!$A$1:$A$3</xm:f>
@@ -3470,26 +3709,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>